<commit_message>
se agrego el sistema de cfdi y nomina timbrado
ademas se cambio el sistema de liquidaciones por un formato un poco mas nuevo
</commit_message>
<xml_diff>
--- a/GeneraReportes/Contratos.xlsx
+++ b/GeneraReportes/Contratos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>Clave Contrato</t>
   </si>
@@ -98,97 +98,100 @@
     <t>2014-12-28</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>DIF</t>
+  </si>
+  <si>
+    <t>11590</t>
+  </si>
+  <si>
+    <t>FID001ADV1014</t>
+  </si>
+  <si>
+    <t>ADMINISTRACIÓN Y DESARROLLO DEL VALOR HUMANO, S. DE R.L. DE C.V.</t>
+  </si>
+  <si>
+    <t>PRINCIPAL</t>
+  </si>
+  <si>
+    <t>ADEVALH</t>
+  </si>
+  <si>
+    <t>MICHOACAN #550 ALTOS, COLONIA RODRIGUEZ, REYNOSA, TAMAULIPAS, C.P. 88630, MEXICO</t>
+  </si>
+  <si>
+    <t>ADV120130IM2</t>
+  </si>
+  <si>
+    <t>(899) 922 7001</t>
+  </si>
+  <si>
+    <t>JACOBO-VALENZUELA@GP.ORG.MX</t>
+  </si>
+  <si>
+    <t>5071</t>
+  </si>
+  <si>
+    <t>TAM</t>
+  </si>
+  <si>
+    <t>88630</t>
+  </si>
+  <si>
+    <t>FID002ATO1014</t>
+  </si>
+  <si>
+    <t>ADMINISTRACIÓN DEL TALENTO ORGANIZACIONAL, S.A. DE C.V.</t>
+  </si>
+  <si>
+    <t>MICHOACAN #550, COLONIA RODRIGUEZ, REYNOSA, TAMAULIPAS, C.P. 88630, MEXICO</t>
+  </si>
+  <si>
+    <t>ATO1201044I0</t>
+  </si>
+  <si>
+    <t>(899) 922 7000</t>
+  </si>
+  <si>
+    <t>5072</t>
+  </si>
+  <si>
+    <t>FID003RST0916</t>
+  </si>
+  <si>
+    <t>RETRO STUDIO, S.C.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>AVE BENJAMIN FRANKLIN # 233, PISO 4, HIPODROMO DE LA CONDESA, CUAUHTEMOC, 06170</t>
+  </si>
+  <si>
+    <t>RST070309F47</t>
+  </si>
+  <si>
+    <t>52776158</t>
+  </si>
+  <si>
+    <t>VERONICA.MORENO@GARANTE.MX</t>
+  </si>
+  <si>
+    <t>PATRIMONIO</t>
+  </si>
+  <si>
+    <t>MÉXICO</t>
+  </si>
+  <si>
+    <t>2015-12-27</t>
+  </si>
+  <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>DIF</t>
-  </si>
-  <si>
-    <t>11590</t>
-  </si>
-  <si>
-    <t>FID001ADV1014</t>
-  </si>
-  <si>
-    <t>ADMINISTRACIÓN Y DESARROLLO DEL VALOR HUMANO, S. DE R.L. DE C.V.</t>
-  </si>
-  <si>
-    <t>PRINCIPAL</t>
-  </si>
-  <si>
-    <t>ADEVALH</t>
-  </si>
-  <si>
-    <t>MICHOACAN #550 ALTOS, COLONIA RODRIGUEZ, REYNOSA, TAMAULIPAS, C.P. 88630, MEXICO</t>
-  </si>
-  <si>
-    <t>ADV120130IM2</t>
-  </si>
-  <si>
-    <t>(899) 922 7001</t>
-  </si>
-  <si>
-    <t>JACOBO-VALENZUELA@GP.ORG.MX</t>
-  </si>
-  <si>
-    <t>5071</t>
-  </si>
-  <si>
-    <t>TAM</t>
-  </si>
-  <si>
-    <t>88630</t>
-  </si>
-  <si>
-    <t>FID002ATO1014</t>
-  </si>
-  <si>
-    <t>ADMINISTRACIÓN DEL TALENTO ORGANIZACIONAL, S.A. DE C.V.</t>
-  </si>
-  <si>
-    <t>MICHOACAN #550, COLONIA RODRIGUEZ, REYNOSA, TAMAULIPAS, C.P. 88630, MEXICO</t>
-  </si>
-  <si>
-    <t>ATO1201044I0</t>
-  </si>
-  <si>
-    <t>(899) 922 7000</t>
-  </si>
-  <si>
-    <t>5072</t>
-  </si>
-  <si>
-    <t>FID003RST0916</t>
-  </si>
-  <si>
-    <t>RETRO STUDIO, S.C.</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>AVE BENJAMIN FRANKLIN # 233, PISO 4, HIPODROMO DE LA CONDESA, CUAUHTEMOC, 06170</t>
-  </si>
-  <si>
-    <t>RST070309F47</t>
-  </si>
-  <si>
-    <t>52776158</t>
-  </si>
-  <si>
-    <t>VERONICA.MORENO@GARANTE.MX</t>
-  </si>
-  <si>
-    <t>PATRIMONIO</t>
-  </si>
-  <si>
-    <t>MÉXICO</t>
-  </si>
-  <si>
-    <t>2015-12-27</t>
   </si>
   <si>
     <t>5557</t>
@@ -389,7 +392,7 @@
     <col min="11" max="11" width="10.23828125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="13.875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="6.58984375" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="8.28125" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="5.921875" customWidth="true" bestFit="true"/>
     <col min="15" max="15" width="8.88671875" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="17.8359375" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="13.17578125" customWidth="true" bestFit="true"/>
@@ -645,19 +648,19 @@
         <v>58</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="N5" s="18" t="n">
-        <v>1565.01</v>
+        <v>0.0</v>
       </c>
       <c r="O5" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P5" s="18" t="s">
         <v>30</v>
       </c>
       <c r="Q5" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>